<commit_message>
Leading empty rows or columns are no longer skipped.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/example2.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/example2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="first_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">The data is on the next sheet </t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">2011Q2</t>
   </si>
   <si>
+    <t xml:space="preserve">zz</t>
+  </si>
+  <si>
     <t xml:space="preserve">this is a complex test fie</t>
   </si>
   <si>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">Timeseries b in euros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxxx</t>
   </si>
   <si>
     <t xml:space="preserve">b</t>
@@ -182,7 +188,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="114.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,22 +212,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.76530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.56632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -234,21 +240,24 @@
       <c r="H1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -262,18 +271,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>10</v>

</xml_diff>